<commit_message>
add generalised table and combined plot year round 8th MARCH
</commit_message>
<xml_diff>
--- a/stats/austroplaca/month_temp_stats_X3.xlsx
+++ b/stats/austroplaca/month_temp_stats_X3.xlsx
@@ -637,9 +637,15 @@
       <c r="B17" t="n">
         <v>2</v>
       </c>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
+      <c r="C17" t="n">
+        <v>-7.35543964232488</v>
+      </c>
+      <c r="D17" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-15.9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>